<commit_message>
Update predictions for vijay
</commit_message>
<xml_diff>
--- a/predictions_vijay.xlsx
+++ b/predictions_vijay.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,22 +458,44 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>22-03-2025</t>
+          <t>23-03-2025</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Kolkata Knight Riders vs Royal Challengers Bengaluru</t>
+          <t>Sunrisers Hyderabad vs Rajasthan Royals</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Royal Challengers Bengaluru</t>
+          <t>Sunrisers Hyderabad</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Royal Challengers Bengaluru</t>
+          <t>Sunrisers Hyderabad</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>23-03-2025</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Chennai Super Kings vs Mumbai Indians</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Chennai Super Kings</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Chennai Super Kings</t>
         </is>
       </c>
     </row>

</xml_diff>